<commit_message>
Cobranza por cabeceras Base
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Cobranza por Prestaciones/Cobranza por Cabeceras/tabla_parametros_comprobantes _test.xlsx
+++ b/DBA/Reportes BI/2021/Cobranza por Prestaciones/Cobranza por Cabeceras/tabla_parametros_comprobantes _test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>FACA2</t>
   </si>
@@ -59,24 +59,6 @@
     <t>Comprobante</t>
   </si>
   <si>
-    <t>FACASIA</t>
-  </si>
-  <si>
-    <t>FACASIB</t>
-  </si>
-  <si>
-    <t>NDAASI</t>
-  </si>
-  <si>
-    <t>NDBASI</t>
-  </si>
-  <si>
-    <t>NOTADB</t>
-  </si>
-  <si>
-    <t>notadb</t>
-  </si>
-  <si>
     <t>NCA</t>
   </si>
   <si>
@@ -86,13 +68,22 @@
     <t>NCECA</t>
   </si>
   <si>
-    <t>otro</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>RECX2</t>
+  </si>
+  <si>
+    <t>tipo2</t>
+  </si>
+  <si>
+    <t>notadebito</t>
+  </si>
+  <si>
+    <t>notacredito</t>
+  </si>
+  <si>
+    <t>recibo</t>
   </si>
 </sst>
 </file>
@@ -222,7 +213,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -274,11 +268,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabla_parametros_comprobantes" displayName="tabla_parametros_comprobantes" ref="A1:B18" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="2" name="Comprobante" dataDxfId="1"/>
-    <tableColumn id="1" name="tipo" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabla_parametros_comprobantes" displayName="tabla_parametros_comprobantes" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C13"/>
+  <tableColumns count="3">
+    <tableColumn id="2" name="Comprobante" dataDxfId="2"/>
+    <tableColumn id="1" name="tipo" dataDxfId="1"/>
+    <tableColumn id="3" name="tipo2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,16 +542,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -566,6 +562,9 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -574,6 +573,9 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -583,6 +585,9 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -591,6 +596,9 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -599,6 +607,9 @@
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -607,6 +618,9 @@
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -615,6 +629,9 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -623,6 +640,9 @@
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -631,21 +651,30 @@
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -653,55 +682,21 @@
         <v>13</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>